<commit_message>
minor cosmetic changes and readme
</commit_message>
<xml_diff>
--- a/mouse2joystick_citra_keylist_automation.xlsx
+++ b/mouse2joystick_citra_keylist_automation.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thinker\Desktop\citra-windows-msvc-20170528-3df85a1\mouse2joystick_citra\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thinker\Desktop\citra-windows-msvc-20170528-3df85a1\mouse2joystick_citra-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -188,9 +188,6 @@
     <t>d</t>
   </si>
   <si>
-    <t>Paste the line below into mouse2joystick's keylist:</t>
-  </si>
-  <si>
     <t>Game 2</t>
   </si>
   <si>
@@ -201,6 +198,9 @@
   </si>
   <si>
     <t>(The other 3 lists are optional for other games)</t>
+  </si>
+  <si>
+    <t>Paste the line below into mouse2joystick_citra's keylist:</t>
   </si>
 </sst>
 </file>
@@ -454,14 +454,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="7">
     <dxf>
       <fill>
         <patternFill>
@@ -824,7 +817,7 @@
   <dimension ref="B1:K42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -860,7 +853,7 @@
         <v>34</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -874,7 +867,7 @@
         <v>12</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="H3" s="6" t="s">
         <v>11</v>
@@ -937,7 +930,7 @@
         <v>10</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H6" s="10" t="s">
         <v>7</v>
@@ -1222,13 +1215,13 @@
         <v>34</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>34</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="24" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>